<commit_message>
Fixed bugs and improved.
</commit_message>
<xml_diff>
--- a/playground/doc/TestControl.xlsx
+++ b/playground/doc/TestControl.xlsx
@@ -9,12 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="state-chart" sheetId="1" r:id="rId1"/>
-    <sheet name="itemsinfo" sheetId="10" r:id="rId13"/>
-    <sheet name="help" sheetId="9" r:id="rId12"/>
-    <sheet name="setting.ini" sheetId="8" r:id="rId11"/>
-    <sheet name="template-statefunc" sheetId="7" r:id="rId10"/>
-    <sheet name="template-source" sheetId="6" r:id="rId9"/>
-    <sheet name="config" sheetId="5" r:id="rId8"/>
+    <sheet name="itemsinfo" sheetId="52" r:id="rId55"/>
+    <sheet name="help" sheetId="51" r:id="rId54"/>
+    <sheet name="setting.ini" sheetId="50" r:id="rId53"/>
+    <sheet name="template-statefunc" sheetId="49" r:id="rId52"/>
+    <sheet name="template-source" sheetId="48" r:id="rId51"/>
+    <sheet name="config" sheetId="47" r:id="rId50"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>state</t>
     <phoneticPr fontId="2"/>
@@ -298,21 +298,21 @@
 gendir=C:\Users\gea01\Documents\psgg\samples\psgg-javascript-sample\playground\public\js
 genrdir=..\public\js
 incrdir=.
-code_output_start=[SYN-G-GEN OUTPUT START]
-code_output_end=[SYN-G-GEN OUTPUT END]
+code_output_start=[STATEGO OUTPUT START]
+code_output_end=[STATEGO OUTPUT END]
 [macro]
 ; This section has macro defines for converting.
 ; commentline format  {%0} will be replaced to a comment.
 commentline=// {%0}
 @branch=@@@
 &lt;&lt;&lt;?"{%0}"/^brifc{0,1}$/
-if ([[brcond:{%N}]]) { this.setnext( this.{%1} ); }
+if ([[brcond:{%N}]]) { this.goto( this.{%1} ); }
 &gt;&gt;&gt;
 &lt;&lt;&lt;?"{%0}"/^brelseifc{0,1}$/
-else if ([[brcond:{%N}]]) { this.setnext( this.{%1} ); }
+else if ([[brcond:{%N}]]) { this.goto( this.{%1} ); }
 &gt;&gt;&gt;
 &lt;&lt;&lt;?"{%0}"/^brelse$/
-else { this.setnext( this.{%1} ); }
+else { this.goto( this.{%1} ); }
 &gt;&gt;&gt;
 &lt;&lt;&lt;?"{%0}"/^br_/
 this.{%0}( this.{%1} );
@@ -379,10 +379,13 @@
     <t>(bitmap)</t>
   </si>
   <si>
-    <t>new state</t>
-  </si>
-  <si>
-    <t>alert("!");</t>
+    <t>S_0002</t>
+  </si>
+  <si>
+    <t>S_0003</t>
+  </si>
+  <si>
+    <t>this.node_xx.innerHTML = 'HOGE HOGE GAA';</t>
   </si>
   <si>
     <t>/
@@ -390,14 +393,93 @@
 </t>
   </si>
   <si>
-    <t>218,259</t>
+    <t>50,439</t>
   </si>
   <si>
     <t>100003</t>
   </si>
   <si>
-    <t>; The setting was created automatically. 2019/04/17 23:05:19
-; * pssgEditor version : 0.51.1337.973e447d167910305e637b16a7bdd1baa4ae7a6e
+    <t>S_0004</t>
+  </si>
+  <si>
+    <t>this.counter = 0;</t>
+  </si>
+  <si>
+    <t>48,571</t>
+  </si>
+  <si>
+    <t>100004</t>
+  </si>
+  <si>
+    <t>ADD IMAGE</t>
+  </si>
+  <si>
+    <t>S_0005</t>
+  </si>
+  <si>
+    <t>const c = document.createElement('div');
+c.id = 'container';
+c.innerHTML = '&lt;img src = "http://statego.programanic.com/img/sgg.png" width="100px"&gt;&lt;/imsg&gt;';
+document.body.appendChild(c);</t>
+  </si>
+  <si>
+    <t>298,488</t>
+  </si>
+  <si>
+    <t>100005</t>
+  </si>
+  <si>
+    <t>wait 2 sec</t>
+  </si>
+  <si>
+    <t>S_0006</t>
+  </si>
+  <si>
+    <t>this.timer = Date.now() + 2000;
+</t>
+  </si>
+  <si>
+    <t>Date.now() &lt; this.timmer</t>
+  </si>
+  <si>
+    <t>536,494</t>
+  </si>
+  <si>
+    <t>100006</t>
+  </si>
+  <si>
+    <t>this.counter++;</t>
+  </si>
+  <si>
+    <t>brifc(S_0004);
+brelse(S_END);</t>
+  </si>
+  <si>
+    <t>?
+?</t>
+  </si>
+  <si>
+    <t>this.counter &lt; 5
+?</t>
+  </si>
+  <si>
+    <t>754,493</t>
+  </si>
+  <si>
+    <t>100007</t>
+  </si>
+  <si>
+    <t>this.node_xx = document.getElementById('xx');</t>
+  </si>
+  <si>
+    <t>56,252</t>
+  </si>
+  <si>
+    <t>100008</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:27:39
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
 psggfile=@@@
 TestControl.psgg
 @@@
@@ -405,7 +487,7 @@
 TestControl.xlsx
 @@@
 guid=@@@
-c876cd6d-5fa5-4dc0-8522-0b6baae509d8
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
 @@@
 bitmap_width=5000
 bitmap_height=2000
@@ -414,7 +496,7 @@
 c_contents=1
 force_display_outpin=0
 last_action=@@@
-Edited a state.
+Changed an arrow direction
 @@@
 target_pathdir=@@@
 /
@@ -428,7 +510,7 @@
 []
 @@@
 fillter_state_location_list=@@@
-[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0001","Value":{"x":218,"y":259}}]}]
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":536,"y":494}},{"Key":"S_0006","Value":{"x":754,"y":493}},{"Key":"S_0001","Value":{"x":56,"y":252}}]}]
 @@@
 linecolor_data=@@@
 [{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
@@ -474,6 +556,605 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Date.now() &lt; this.timer</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:28:40
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Edited a state.
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":536,"y":494}},{"Key":"S_0006","Value":{"x":754,"y":493}},{"Key":"S_0001","Value":{"x":56,"y":252}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>brifc(S_0004);
+brelse(S_0008);</t>
+  </si>
+  <si>
+    <t>S_0007</t>
+  </si>
+  <si>
+    <t>new state</t>
+  </si>
+  <si>
+    <t>1055,266</t>
+  </si>
+  <si>
+    <t>100009</t>
+  </si>
+  <si>
+    <t>S_0008</t>
+  </si>
+  <si>
+    <t>const c = document.createElement('div');
+c.id = 'container';
+c.innerHTML = '&lt;img src = "http://statego.programanic.com/img/sgg.png"&gt;&lt;/imsg&gt;';
+document.body.appendChild(c);</t>
+  </si>
+  <si>
+    <t>/
+(0,0)
+</t>
+  </si>
+  <si>
+    <t>1043,466</t>
+  </si>
+  <si>
+    <t>100010</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:31:40
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Edited a state.
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":536,"y":494}},{"Key":"S_0006","Value":{"x":754,"y":493}},{"Key":"S_0001","Value":{"x":56,"y":252}},{"Key":"S_0007","Value":{"x":1055,"y":266}},{"Key":"S_0008","Value":{"x":1043,"y":466}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:31:44
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Edited a state.
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":536,"y":494}},{"Key":"S_0006","Value":{"x":754,"y":493}},{"Key":"S_0001","Value":{"x":56,"y":252}},{"Key":"S_0007","Value":{"x":1055,"y":266}},{"Key":"S_0008","Value":{"x":1043,"y":466}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>const c = document.createElement('span');
+c.id = 'container';
+c.innerHTML = '&lt;img src = "http://statego.programanic.com/img/sgg.png" width="100px"&gt;&lt;/img&gt;';
+document.body.appendChild(c);</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:32:31
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Edited a state.
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":536,"y":494}},{"Key":"S_0006","Value":{"x":754,"y":493}},{"Key":"S_0001","Value":{"x":56,"y":252}},{"Key":"S_0007","Value":{"x":1055,"y":266}},{"Key":"S_0008","Value":{"x":1043,"y":466}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>ADD SMALL IMAGE</t>
+  </si>
+  <si>
+    <t>529,657</t>
+  </si>
+  <si>
+    <t>759,505</t>
+  </si>
+  <si>
+    <t>1147,476</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:33:59
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Edited a state.
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":529,"y":657}},{"Key":"S_0006","Value":{"x":759,"y":505}},{"Key":"S_0001","Value":{"x":56,"y":252}},{"Key":"S_0007","Value":{"x":1055,"y":266}},{"Key":"S_0008","Value":{"x":1147,"y":476}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>532,530</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:34:15
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Moved a state
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":532,"y":530}},{"Key":"S_0006","Value":{"x":759,"y":505}},{"Key":"S_0001","Value":{"x":56,"y":252}},{"Key":"S_0007","Value":{"x":1055,"y":266}},{"Key":"S_0008","Value":{"x":1147,"y":476}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/20 9:34:40
+; * pssgEditor version : 0.51.8581.08cb3e34869684c0da626d3d3a25e0c946eef1cf
+psggfile=@@@
+TestControl.psgg
+@@@
+xlsfile=@@@
+TestControl.xlsx
+@@@
+guid=@@@
+d90ae5a9-ad00-4e6c-8eaf-e11ae54de063
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Moved a state
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[]
+@@@
+nodegroup_pos_list=@@@
+[]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":50,"y":100}},{"Key":"S_END","Value":{"x":312,"y":100}},{"Key":"S_0002","Value":{"x":50,"y":439}},{"Key":"S_0003","Value":{"x":48,"y":571}},{"Key":"S_0004","Value":{"x":298,"y":488}},{"Key":"S_0005","Value":{"x":532,"y":530}},{"Key":"S_0006","Value":{"x":759,"y":505}},{"Key":"S_0001","Value":{"x":56,"y":252}},{"Key":"S_0007","Value":{"x":1055,"y":266}},{"Key":"S_0008","Value":{"x":1147,"y":476}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=1
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=45
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1697,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="false" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1043,6 +1724,24 @@
       <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" s="4" customFormat="true">
       <c r="A2" s="3"/>
@@ -1059,7 +1758,28 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" s="7" customFormat="true">
@@ -1072,8 +1792,17 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="5" t="s">
-        <v>37</v>
+      <c r="H3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" s="7" customFormat="true">
@@ -1098,6 +1827,21 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1142,7 +1886,25 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" s="11" customFormat="true">
@@ -1203,6 +1965,9 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
+      <c r="I17" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="18" s="11" customFormat="true">
       <c r="A18" s="10"/>
@@ -1253,6 +2018,9 @@
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
+      <c r="J23" s="12" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="24" s="13" customFormat="true">
       <c r="A24" s="12"/>
@@ -1262,6 +2030,9 @@
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
+      <c r="J24" s="12" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" s="13" customFormat="true">
       <c r="A25" s="12"/>
@@ -1271,6 +2042,9 @@
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
+      <c r="J25" s="12" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="26" s="15" customFormat="true" ht="18.75" customHeight="true">
       <c r="A26" s="14"/>
@@ -1280,6 +2054,15 @@
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
+      <c r="H26" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" s="16" customFormat="true"/>
     <row r="28" s="16" customFormat="true">
@@ -1287,7 +2070,28 @@
         <v>16</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" s="16" customFormat="true">
@@ -1301,7 +2105,28 @@
         <v>33</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" s="16" customFormat="true">
@@ -1315,7 +2140,28 @@
         <v>35</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1325,49 +2171,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1381,7 +2213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1395,7 +2227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1407,4 +2239,18 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>